<commit_message>
mail level code for failure
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="7">
   <si>
     <t>Mail Level</t>
   </si>
@@ -997,7 +997,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1013,7 +1013,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pay button xpath change
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="7">
   <si>
     <t>Mail Level</t>
   </si>
@@ -997,7 +997,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1005,7 +1005,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1013,7 +1013,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pay button code change
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="7">
   <si>
     <t>Mail Level</t>
   </si>
@@ -997,7 +997,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1005,7 +1005,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>